<commit_message>
Atualizacao automatica do sistema
</commit_message>
<xml_diff>
--- a/usuarios_backup.xlsx
+++ b/usuarios_backup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriele\Documents\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A6A67AC5-9E50-4818-9BE6-943A9995E40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4794E7F7-93D2-4182-8636-4CBA072673AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D2EC7CC-EF8C-45E6-A144-D8508B2658A9}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Data</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Cargo</t>
+  </si>
+  <si>
+    <t>rother</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -895,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC141FEE-1D2F-4E3F-9491-30E9FBAC44AD}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,6 +929,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>784512</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>